<commit_message>
Added test results to FPU-calc.xlsx
</commit_message>
<xml_diff>
--- a/FPU-calc.xlsx
+++ b/FPU-calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="760" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="2780" yWindow="280" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Enter Fat</t>
   </si>
@@ -67,6 +67,48 @@
   </si>
   <si>
     <t>hrs for manual pump</t>
+  </si>
+  <si>
+    <t>carb</t>
+  </si>
+  <si>
+    <t>fat</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>bolus</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Note - duration should be entered as 4 hrs minimum for manual pump</t>
+  </si>
+  <si>
+    <t>or 7 hours minimum for Loop or OpenAPS.</t>
+  </si>
+  <si>
+    <t>Verification tests:</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected </t>
   </si>
 </sst>
 </file>
@@ -76,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +149,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -131,7 +185,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -139,21 +193,82 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C14"/>
+  <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,108 +610,421 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3">
+    <row r="2" spans="1:14">
+      <c r="G2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="F4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <f>(B4/80)+0.5</f>
-        <v>1.125</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="F9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>45</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3">
         <f>((B5*9+B6*4)/B9)*10</f>
-        <v>82</v>
+        <v>57.5</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>9.5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="3">
         <f>B11*B8</f>
-        <v>92.25</v>
+        <v>57.5</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="G12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <f>((B5*9+B6*4)/B9)+2</f>
-        <v>10.199999999999999</v>
+        <v>7.75</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4">
         <f>B13+3</f>
-        <v>13.2</v>
+        <v>10.75</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="F15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18">
+        <v>80</v>
+      </c>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="M18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="F20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="G23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>